<commit_message>
Add local files before rebase
</commit_message>
<xml_diff>
--- a/Balamurali V_test_cast_design_for_redif_account_creation.xlsx
+++ b/Balamurali V_test_cast_design_for_redif_account_creation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bala\HCL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9DE7219-4C37-4C45-B941-8F33D7CA254D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62A2F12-7CCD-4ADA-ABAA-E2434FDA6126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenario" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="211">
   <si>
     <t>Test Scenario</t>
   </si>
@@ -156,9 +156,6 @@
     <t>ScreenShot</t>
   </si>
   <si>
-    <t>Reddit</t>
-  </si>
-  <si>
     <t>v0.0.1</t>
   </si>
   <si>
@@ -577,6 +574,93 @@
   </si>
   <si>
     <t>The entered captcha should be displayed in the "CAPTCHA"field</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>The error message should be "Enter valid Mobile number"</t>
+  </si>
+  <si>
+    <t>DEF_001</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>TC_003</t>
+  </si>
+  <si>
+    <t>TC_006</t>
+  </si>
+  <si>
+    <t>TC_007</t>
+  </si>
+  <si>
+    <t>TC_008</t>
+  </si>
+  <si>
+    <t>TC_009</t>
+  </si>
+  <si>
+    <t>TC_010</t>
+  </si>
+  <si>
+    <t>TC_011</t>
+  </si>
+  <si>
+    <t>TC_012,TC_013</t>
+  </si>
+  <si>
+    <t>COVERED</t>
+  </si>
+  <si>
+    <t>NOT-COVERED</t>
+  </si>
+  <si>
+    <t>TS_001</t>
+  </si>
+  <si>
+    <t>REQ_001</t>
+  </si>
+  <si>
+    <t>REQ_002</t>
+  </si>
+  <si>
+    <t>REQ_003</t>
+  </si>
+  <si>
+    <t>REQ_004</t>
+  </si>
+  <si>
+    <t>REQ_005</t>
+  </si>
+  <si>
+    <t>REQ_006</t>
+  </si>
+  <si>
+    <t>REQ_007</t>
+  </si>
+  <si>
+    <t>REQ_008</t>
+  </si>
+  <si>
+    <t>REQ_009</t>
+  </si>
+  <si>
+    <t>REQ_010</t>
+  </si>
+  <si>
+    <t>REQ_011</t>
+  </si>
+  <si>
+    <t>REQ_012</t>
+  </si>
+  <si>
+    <t>Rediff</t>
   </si>
 </sst>
 </file>
@@ -587,7 +671,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -645,8 +729,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -681,6 +779,16 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -844,14 +952,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -965,9 +1075,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -981,6 +1088,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1027,7 +1140,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1310,7 +1425,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1638,36 +1753,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="51"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="52"/>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="54"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="55"/>
     </row>
     <row r="3" spans="1:5" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="55"/>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
+      <c r="A3" s="56"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
     </row>
     <row r="4" spans="1:5" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="57" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="58"/>
+      <c r="B4" s="58" t="s">
+        <v>210</v>
+      </c>
+      <c r="C4" s="59"/>
       <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1680,7 +1795,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="1" t="s">
@@ -1695,7 +1810,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -1713,7 +1828,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1735,16 +1850,16 @@
     </row>
     <row r="10" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>48</v>
       </c>
       <c r="E10" s="6"/>
     </row>
@@ -1818,8 +1933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H138" sqref="H138"/>
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2787,36 +2902,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
     </row>
     <row r="3" spans="1:12" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="B3" s="55"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
     </row>
     <row r="4" spans="1:12" ht="25.8" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="57" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="58"/>
+      <c r="C4" s="58" t="s">
+        <v>210</v>
+      </c>
+      <c r="D4" s="59"/>
       <c r="E4" s="37" t="s">
         <v>2</v>
       </c>
@@ -2829,7 +2944,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="37" t="s">
@@ -2844,7 +2959,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="37" t="s">
@@ -2864,7 +2979,7 @@
         <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
@@ -2904,28 +3019,32 @@
     </row>
     <row r="10" spans="1:12" s="9" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" s="32">
         <v>1</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="10"/>
+      <c r="H10" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J10" s="10"/>
       <c r="L10" s="30"/>
     </row>
@@ -2935,16 +3054,20 @@
       <c r="C11" s="32"/>
       <c r="D11" s="13"/>
       <c r="E11" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="G11" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="10"/>
+      <c r="H11" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J11" s="10"/>
       <c r="L11" s="30"/>
     </row>
@@ -2954,16 +3077,20 @@
       <c r="C12" s="32"/>
       <c r="D12" s="13"/>
       <c r="E12" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F12" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="10"/>
+      <c r="H12" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="I12" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J12" s="10"/>
       <c r="L12" s="30"/>
     </row>
@@ -2973,13 +3100,19 @@
       <c r="C13" s="17"/>
       <c r="D13" s="10"/>
       <c r="E13" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F13" s="40" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="48" t="s">
+        <v>183</v>
       </c>
       <c r="L13" s="30"/>
     </row>
@@ -2989,13 +3122,19 @@
       <c r="C14" s="32"/>
       <c r="D14" s="13"/>
       <c r="E14" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F14" s="36">
         <v>37897</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="48" t="s">
+        <v>183</v>
       </c>
       <c r="L14" s="30"/>
     </row>
@@ -3005,13 +3144,19 @@
       <c r="C15" s="32"/>
       <c r="D15" s="13"/>
       <c r="E15" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>55</v>
+      <c r="H15" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="48" t="s">
+        <v>183</v>
       </c>
       <c r="L15" s="30"/>
     </row>
@@ -3021,13 +3166,19 @@
       <c r="C16" s="32"/>
       <c r="D16" s="13"/>
       <c r="E16" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F16" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="G16" s="20" t="s">
-        <v>70</v>
+      <c r="H16" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="I16" s="48" t="s">
+        <v>183</v>
       </c>
       <c r="L16" s="30"/>
     </row>
@@ -3037,13 +3188,19 @@
       <c r="C17" s="32"/>
       <c r="D17" s="13"/>
       <c r="E17" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F17" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="G17" s="20" t="s">
-        <v>74</v>
+      <c r="H17" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" s="48" t="s">
+        <v>183</v>
       </c>
       <c r="L17" s="30"/>
     </row>
@@ -3053,13 +3210,19 @@
       <c r="C18" s="17"/>
       <c r="D18" s="10"/>
       <c r="E18" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F18" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="G18" s="20" t="s">
-        <v>76</v>
+      <c r="H18" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="I18" s="48" t="s">
+        <v>183</v>
       </c>
       <c r="L18" s="30"/>
     </row>
@@ -3069,13 +3232,19 @@
       <c r="C19" s="17"/>
       <c r="D19" s="10"/>
       <c r="E19" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F19" s="36">
         <v>123456789</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="I19" s="48" t="s">
+        <v>183</v>
       </c>
       <c r="L19" s="30"/>
     </row>
@@ -3085,11 +3254,17 @@
       <c r="C20" s="32"/>
       <c r="D20" s="13"/>
       <c r="E20" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="I20" s="48" t="s">
+        <v>183</v>
       </c>
       <c r="L20" s="30"/>
     </row>
@@ -3099,37 +3274,49 @@
       <c r="C21" s="32"/>
       <c r="D21" s="13"/>
       <c r="E21" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F21" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G21" s="20" t="s">
-        <v>58</v>
+      <c r="H21" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I21" s="48" t="s">
+        <v>183</v>
       </c>
       <c r="L21" s="30"/>
     </row>
     <row r="22" spans="1:12" s="9" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C22" s="32">
         <v>1</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E22" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="G22" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="F22" s="40" t="s">
-        <v>85</v>
-      </c>
-      <c r="G22" s="20" t="s">
-        <v>51</v>
+      <c r="H22" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="I22" s="48" t="s">
+        <v>183</v>
       </c>
       <c r="L22" s="30"/>
     </row>
@@ -3139,13 +3326,19 @@
       <c r="C23" s="32"/>
       <c r="D23" s="13"/>
       <c r="E23" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F23" s="35" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="H23" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="I23" s="48" t="s">
+        <v>183</v>
       </c>
       <c r="L23" s="30"/>
     </row>
@@ -3155,13 +3348,19 @@
       <c r="C24" s="17"/>
       <c r="D24" s="13"/>
       <c r="E24" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="H24" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="I24" s="48" t="s">
+        <v>183</v>
       </c>
       <c r="L24" s="30"/>
     </row>
@@ -3171,13 +3370,19 @@
       <c r="C25" s="32"/>
       <c r="D25" s="13"/>
       <c r="E25" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G25" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="H25" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="I25" s="48" t="s">
+        <v>183</v>
       </c>
       <c r="L25" s="30"/>
     </row>
@@ -3187,13 +3392,19 @@
       <c r="C26" s="17"/>
       <c r="D26" s="13"/>
       <c r="E26" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F26" s="41">
+        <v>37898</v>
+      </c>
+      <c r="G26" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="F26" s="42">
-        <v>37898</v>
-      </c>
-      <c r="G26" s="20" t="s">
-        <v>53</v>
+      <c r="H26" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="I26" s="48" t="s">
+        <v>183</v>
       </c>
       <c r="L26" s="30"/>
     </row>
@@ -3203,13 +3414,19 @@
       <c r="C27" s="32"/>
       <c r="D27" s="13"/>
       <c r="E27" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G27" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="F27" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="G27" s="20" t="s">
-        <v>55</v>
+      <c r="H27" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="I27" s="48" t="s">
+        <v>183</v>
       </c>
       <c r="L27" s="30"/>
     </row>
@@ -3219,13 +3436,19 @@
       <c r="C28" s="32"/>
       <c r="D28" s="13"/>
       <c r="E28" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F28" s="36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="H28" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="I28" s="48" t="s">
+        <v>183</v>
       </c>
       <c r="L28" s="30"/>
     </row>
@@ -3235,13 +3458,19 @@
       <c r="C29" s="17"/>
       <c r="D29" s="10"/>
       <c r="E29" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F29" s="36" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G29" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="H29" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="I29" s="48" t="s">
+        <v>183</v>
       </c>
       <c r="L29" s="30"/>
     </row>
@@ -3251,13 +3480,19 @@
       <c r="C30" s="32"/>
       <c r="D30" s="13"/>
       <c r="E30" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F30" s="35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G30" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="H30" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="I30" s="48" t="s">
+        <v>183</v>
       </c>
       <c r="L30" s="30"/>
     </row>
@@ -3267,13 +3502,19 @@
       <c r="C31" s="32"/>
       <c r="D31" s="13"/>
       <c r="E31" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F31" s="17">
         <v>123456789</v>
       </c>
       <c r="G31" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="H31" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="I31" s="48" t="s">
+        <v>183</v>
       </c>
       <c r="L31" s="30"/>
     </row>
@@ -3283,11 +3524,17 @@
       <c r="C32" s="17"/>
       <c r="D32" s="10"/>
       <c r="E32" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F32" s="36"/>
       <c r="G32" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="H32" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="I32" s="48" t="s">
+        <v>183</v>
       </c>
       <c r="L32" s="30"/>
     </row>
@@ -3297,55 +3544,70 @@
       <c r="C33" s="32"/>
       <c r="D33" s="13"/>
       <c r="E33" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F33" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G33" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G33" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="H33" s="41"/>
+      <c r="H33" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I33" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="L33" s="30"/>
     </row>
     <row r="34" spans="1:12" s="9" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C34" s="17">
         <v>2</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F34" s="17"/>
       <c r="G34" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="H34" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="I34" s="48" t="s">
+        <v>183</v>
       </c>
       <c r="L34" s="30"/>
     </row>
-    <row r="35" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="32"/>
       <c r="D35" s="13"/>
       <c r="E35" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
+        <v>93</v>
+      </c>
+      <c r="H35" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="I35" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
     </row>
@@ -3355,43 +3617,51 @@
       <c r="C36" s="17"/>
       <c r="D36" s="10"/>
       <c r="E36" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F36" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G36" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G36" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
+      <c r="H36" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I36" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
     </row>
     <row r="37" spans="1:12" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C37" s="32">
         <v>3</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G37" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
+        <v>93</v>
+      </c>
+      <c r="H37" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="I37" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
     </row>
@@ -3401,10 +3671,16 @@
       <c r="C38" s="17"/>
       <c r="D38" s="20"/>
       <c r="E38" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G38" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
+      </c>
+      <c r="H38" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="I38" s="48" t="s">
+        <v>183</v>
       </c>
       <c r="L38" s="30"/>
     </row>
@@ -3413,16 +3689,20 @@
       <c r="B39" s="13"/>
       <c r="C39" s="17"/>
       <c r="E39" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F39" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="G39" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="G39" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
+      <c r="H39" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="I39" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J39" s="9"/>
       <c r="K39" s="9"/>
     </row>
@@ -3431,16 +3711,20 @@
       <c r="B40" s="13"/>
       <c r="C40" s="32"/>
       <c r="E40" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F40" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G40" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="G40" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
+      <c r="H40" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="I40" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J40" s="9"/>
       <c r="K40" s="9"/>
     </row>
@@ -3449,58 +3733,70 @@
       <c r="B41" s="13"/>
       <c r="C41" s="32"/>
       <c r="E41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F41" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="G41" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="G41" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
+      <c r="H41" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="I41" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J41" s="9"/>
       <c r="K41" s="9"/>
     </row>
     <row r="42" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
       <c r="E42" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F42" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G42" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G42" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
+      <c r="H42" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I42" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
     </row>
     <row r="43" spans="1:12" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C43" s="32">
         <v>4</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E43" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G43" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
+        <v>93</v>
+      </c>
+      <c r="H43" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="I43" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J43" s="9"/>
       <c r="K43" s="9"/>
     </row>
@@ -3510,33 +3806,41 @@
       <c r="C44" s="32"/>
       <c r="D44" s="13"/>
       <c r="E44" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F44" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="F44" s="35" t="s">
-        <v>62</v>
-      </c>
       <c r="G44" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
+        <v>101</v>
+      </c>
+      <c r="H44" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="I44" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
     </row>
-    <row r="45" spans="1:12" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A45" s="13"/>
       <c r="B45" s="13"/>
       <c r="C45" s="32"/>
       <c r="D45" s="13"/>
       <c r="E45" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F45" s="9"/>
       <c r="G45" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
+        <v>110</v>
+      </c>
+      <c r="H45" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="I45" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J45" s="9"/>
       <c r="K45" s="9"/>
     </row>
@@ -3546,16 +3850,20 @@
       <c r="C46" s="32"/>
       <c r="D46" s="13"/>
       <c r="E46" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F46" s="35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G46" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
+        <v>112</v>
+      </c>
+      <c r="H46" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="I46" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J46" s="9"/>
       <c r="K46" s="9"/>
     </row>
@@ -3565,12 +3873,14 @@
       <c r="C47" s="32"/>
       <c r="D47" s="13"/>
       <c r="E47" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F47" s="17"/>
       <c r="G47" s="20"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="9"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
     </row>
@@ -3580,58 +3890,70 @@
       <c r="C48" s="32"/>
       <c r="D48" s="13"/>
       <c r="E48" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F48" s="36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G48" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="H48" s="9"/>
-      <c r="I48" s="9"/>
+        <v>112</v>
+      </c>
+      <c r="H48" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="I48" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
     </row>
     <row r="49" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
       <c r="E49" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F49" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G49" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G49" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
+      <c r="H49" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I49" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J49" s="9"/>
       <c r="K49" s="9"/>
     </row>
     <row r="50" spans="1:12" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C50" s="32">
         <v>5</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E50" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F50" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G50" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
+        <v>93</v>
+      </c>
+      <c r="H50" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="I50" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J50" s="9"/>
       <c r="K50" s="9"/>
     </row>
@@ -3641,16 +3963,20 @@
       <c r="C51" s="32"/>
       <c r="D51" s="13"/>
       <c r="E51" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F51" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="F51" s="35" t="s">
-        <v>62</v>
-      </c>
       <c r="G51" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="H51" s="9"/>
-      <c r="I51" s="9"/>
+        <v>101</v>
+      </c>
+      <c r="H51" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="I51" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J51" s="9"/>
       <c r="K51" s="9"/>
     </row>
@@ -3660,16 +3986,20 @@
       <c r="C52" s="32"/>
       <c r="D52" s="13"/>
       <c r="E52" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="F52" s="47" t="s">
-        <v>64</v>
+        <v>118</v>
+      </c>
+      <c r="F52" s="46" t="s">
+        <v>63</v>
       </c>
       <c r="G52" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="H52" s="9"/>
-      <c r="I52" s="9"/>
+        <v>112</v>
+      </c>
+      <c r="H52" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="I52" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J52" s="9"/>
       <c r="K52" s="9"/>
     </row>
@@ -3679,10 +4009,16 @@
       <c r="C53" s="17"/>
       <c r="D53" s="10"/>
       <c r="E53" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="G53" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="G53" s="20" t="s">
-        <v>121</v>
+      <c r="H53" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="I53" s="48" t="s">
+        <v>183</v>
       </c>
       <c r="L53" s="30"/>
     </row>
@@ -3692,16 +4028,20 @@
       <c r="C54" s="32"/>
       <c r="D54" s="13"/>
       <c r="E54" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="F54" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="F54" s="17" t="s">
+      <c r="G54" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="G54" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
+      <c r="H54" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="I54" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J54" s="9"/>
       <c r="K54" s="9"/>
     </row>
@@ -3711,43 +4051,51 @@
       <c r="C55" s="32"/>
       <c r="D55" s="13"/>
       <c r="E55" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F55" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G55" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G55" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="H55" s="9"/>
-      <c r="I55" s="9"/>
+      <c r="H55" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I55" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J55" s="9"/>
       <c r="K55" s="9"/>
     </row>
     <row r="56" spans="1:12" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A56" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C56" s="32">
         <v>6</v>
       </c>
       <c r="D56" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E56" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G56" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="H56" s="9"/>
-      <c r="I56" s="9"/>
+        <v>93</v>
+      </c>
+      <c r="H56" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="I56" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
     </row>
@@ -3757,16 +4105,20 @@
       <c r="C57" s="32"/>
       <c r="D57" s="13"/>
       <c r="E57" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F57" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="F57" s="35" t="s">
-        <v>62</v>
-      </c>
       <c r="G57" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
+        <v>101</v>
+      </c>
+      <c r="H57" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="I57" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
     </row>
@@ -3776,16 +4128,20 @@
       <c r="C58" s="32"/>
       <c r="D58" s="13"/>
       <c r="E58" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="F58" s="47" t="s">
-        <v>64</v>
+        <v>118</v>
+      </c>
+      <c r="F58" s="46" t="s">
+        <v>63</v>
       </c>
       <c r="G58" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="H58" s="9"/>
-      <c r="I58" s="9"/>
+        <v>112</v>
+      </c>
+      <c r="H58" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="I58" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
     </row>
@@ -3795,16 +4151,20 @@
       <c r="C59" s="32"/>
       <c r="D59" s="13"/>
       <c r="E59" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F59" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="G59" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="F59" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="G59" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="H59" s="9"/>
-      <c r="I59" s="9"/>
+      <c r="H59" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="I59" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
     </row>
@@ -3813,17 +4173,21 @@
       <c r="B60" s="13"/>
       <c r="C60" s="32"/>
       <c r="D60" s="13"/>
-      <c r="E60" s="46" t="s">
+      <c r="E60" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G60" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="F60" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="G60" s="46" t="s">
-        <v>129</v>
-      </c>
-      <c r="H60" s="9"/>
-      <c r="I60" s="9"/>
+      <c r="H60" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="I60" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
     </row>
@@ -3833,16 +4197,20 @@
       <c r="C61" s="32"/>
       <c r="D61" s="13"/>
       <c r="E61" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="F61" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="G61" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="F61" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="G61" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="H61" s="9"/>
-      <c r="I61" s="9"/>
+      <c r="H61" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="I61" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J61" s="9"/>
       <c r="K61" s="9"/>
     </row>
@@ -3851,17 +4219,21 @@
       <c r="B62" s="13"/>
       <c r="C62" s="32"/>
       <c r="D62" s="13"/>
-      <c r="E62" s="46" t="s">
+      <c r="E62" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="F62" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G62" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="F62" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="G62" s="46" t="s">
-        <v>133</v>
-      </c>
-      <c r="H62" s="9"/>
-      <c r="I62" s="9"/>
+      <c r="H62" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="I62" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
     </row>
@@ -3871,43 +4243,51 @@
       <c r="C63" s="32"/>
       <c r="D63" s="13"/>
       <c r="E63" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F63" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G63" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G63" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="H63" s="9"/>
-      <c r="I63" s="9"/>
+      <c r="H63" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I63" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
     </row>
     <row r="64" spans="1:12" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C64" s="32">
         <v>7</v>
       </c>
       <c r="D64" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E64" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F64" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G64" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="H64" s="9"/>
-      <c r="I64" s="9"/>
+        <v>93</v>
+      </c>
+      <c r="H64" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="I64" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
     </row>
@@ -3917,13 +4297,19 @@
       <c r="C65" s="17"/>
       <c r="D65" s="10"/>
       <c r="E65" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F65" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="F65" s="35" t="s">
-        <v>62</v>
-      </c>
       <c r="G65" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
+      </c>
+      <c r="H65" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="I65" s="48" t="s">
+        <v>183</v>
       </c>
       <c r="L65" s="30"/>
     </row>
@@ -3933,16 +4319,20 @@
       <c r="C66" s="33"/>
       <c r="D66" s="9"/>
       <c r="E66" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="F66" s="47" t="s">
-        <v>64</v>
+        <v>118</v>
+      </c>
+      <c r="F66" s="46" t="s">
+        <v>63</v>
       </c>
       <c r="G66" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="H66" s="9"/>
-      <c r="I66" s="9"/>
+        <v>112</v>
+      </c>
+      <c r="H66" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="I66" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
     </row>
@@ -3952,873 +4342,1324 @@
       <c r="C67" s="33"/>
       <c r="D67" s="9"/>
       <c r="E67" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F67" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="G67" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="F67" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="G67" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="H67" s="9"/>
-      <c r="I67" s="9"/>
+      <c r="H67" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="I67" s="48" t="s">
+        <v>183</v>
+      </c>
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
     </row>
     <row r="68" spans="1:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="E68" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F68" s="36">
         <v>37897</v>
       </c>
       <c r="G68" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
+      </c>
+      <c r="H68" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="I68" s="48" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="E69" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="F69" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G69" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="F69" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="G69" s="20" t="s">
-        <v>137</v>
+      <c r="H69" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="I69" s="48" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="70" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
       <c r="E70" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F70" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G70" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G70" s="20" t="s">
-        <v>58</v>
+      <c r="H70" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I70" s="48" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C71" s="34">
         <v>8</v>
       </c>
       <c r="D71" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E71" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F71" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G71" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+      <c r="H71" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="I71" s="48" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="E72" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F72" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="F72" s="35" t="s">
-        <v>62</v>
-      </c>
       <c r="G72" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
+      </c>
+      <c r="H72" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="I72" s="48" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="73" spans="1:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="E73" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="F73" s="47" t="s">
-        <v>64</v>
+        <v>118</v>
+      </c>
+      <c r="F73" s="46" t="s">
+        <v>63</v>
       </c>
       <c r="G73" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
+      </c>
+      <c r="H73" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="I73" s="48" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="74" spans="1:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="E74" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F74" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="G74" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="F74" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="G74" s="20" t="s">
-        <v>127</v>
+      <c r="H74" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="I74" s="48" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="75" spans="1:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="E75" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F75" s="36">
         <v>37897</v>
       </c>
       <c r="G75" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
+      </c>
+      <c r="H75" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="I75" s="48" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="76" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
       <c r="E76" s="39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F76" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G76" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
+      </c>
+      <c r="H76" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="I76" s="48" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="77" spans="1:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="E77" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F77" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G77" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
+      </c>
+      <c r="H77" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="I77" s="48" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="78" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
       <c r="E78" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F78" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G78" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G78" s="20" t="s">
-        <v>58</v>
+      <c r="H78" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I78" s="48" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="79" spans="1:12" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C79" s="34">
         <v>9</v>
       </c>
       <c r="D79" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E79" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F79" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G79" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+      <c r="H79" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="I79" s="48" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="80" spans="1:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="E80" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F80" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="F80" s="35" t="s">
-        <v>62</v>
-      </c>
       <c r="G80" s="20" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="H80" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="I80" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="E81" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="F81" s="47" t="s">
-        <v>64</v>
+        <v>118</v>
+      </c>
+      <c r="F81" s="46" t="s">
+        <v>63</v>
       </c>
       <c r="G81" s="20" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+      <c r="H81" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="I81" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="E82" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F82" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="G82" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="F82" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="G82" s="20" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="H82" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="I82" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="E83" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F83" s="36">
         <v>37897</v>
       </c>
       <c r="G83" s="20" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+      <c r="H83" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="I83" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
       <c r="E84" s="39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F84" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G84" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="H84" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="I84" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="E85" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F85" t="s">
+        <v>68</v>
+      </c>
+      <c r="G85" s="20" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="E85" s="20" t="s">
+      <c r="H85" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="I85" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="E86" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="F86" t="s">
         <v>72</v>
       </c>
-      <c r="F85" t="s">
-        <v>69</v>
-      </c>
-      <c r="G85" s="20" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="E86" s="20" t="s">
+      <c r="G86" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="F86" t="s">
-        <v>73</v>
-      </c>
-      <c r="G86" s="20" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="H86" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="I86" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
       <c r="E87" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F87" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G87" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G87" s="20" t="s">
+      <c r="H87" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I87" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>150</v>
+      </c>
+      <c r="B88" s="13" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>151</v>
-      </c>
-      <c r="B88" s="13" t="s">
-        <v>59</v>
       </c>
       <c r="C88" s="34">
         <v>10</v>
       </c>
       <c r="D88" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E88" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F88" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G88" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H88" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="I88" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="E89" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="E88" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="F88" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="G88" s="20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="E89" s="20" t="s">
+      <c r="F89" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="F89" s="35" t="s">
-        <v>62</v>
-      </c>
       <c r="G89" s="20" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="H89" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="I89" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="E90" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="F90" s="47" t="s">
-        <v>64</v>
+        <v>118</v>
+      </c>
+      <c r="F90" s="46" t="s">
+        <v>63</v>
       </c>
       <c r="G90" s="20" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+      <c r="H90" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="I90" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="E91" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F91" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="G91" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="F91" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="G91" s="20" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="H91" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="I91" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="E92" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F92" s="36">
         <v>37897</v>
       </c>
       <c r="G92" s="20" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+      <c r="H92" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="I92" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
       <c r="E93" s="39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F93" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G93" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="H93" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="I93" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="E94" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F94" t="s">
+        <v>68</v>
+      </c>
+      <c r="G94" s="20" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="E94" s="20" t="s">
+      <c r="H94" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="I94" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="E95" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="F95" t="s">
         <v>72</v>
       </c>
-      <c r="F94" t="s">
-        <v>69</v>
-      </c>
-      <c r="G94" s="20" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="E95" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="F95" t="s">
-        <v>73</v>
-      </c>
       <c r="G95" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="H95" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="I95" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="E96" s="20" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="E96" s="20" t="s">
+      <c r="G96" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="G96" s="20" t="s">
+      <c r="H96" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="I96" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E97" s="44" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="E97" s="45" t="s">
+      <c r="F97" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="G97" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="F97" s="48" t="s">
+      <c r="H97" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="I97" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="E98" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="F98" t="s">
         <v>56</v>
       </c>
-      <c r="G97" s="39" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="E98" s="39" t="s">
+      <c r="G98" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="F98" t="s">
+      <c r="H98" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="I98" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="E99" s="45" t="s">
+        <v>156</v>
+      </c>
+      <c r="G99" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="H99" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="I99" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E100" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="G100" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="H100" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="I100" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="E101" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="F101" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G101" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G98" s="39" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="E99" s="46" t="s">
-        <v>157</v>
-      </c>
-      <c r="G99" s="39" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="E100" s="39" t="s">
-        <v>158</v>
-      </c>
-      <c r="G100" s="20" t="s">
+      <c r="H101" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I101" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="E101" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="F101" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G101" s="20" t="s">
+      <c r="B102" s="13" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>156</v>
-      </c>
-      <c r="B102" s="13" t="s">
-        <v>59</v>
       </c>
       <c r="C102" s="34">
         <v>11</v>
       </c>
       <c r="D102" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E102" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F102" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G102" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H102" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="I102" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="E103" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="E102" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="F102" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="G102" s="20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="E103" s="20" t="s">
+      <c r="F103" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="F103" s="35" t="s">
-        <v>62</v>
-      </c>
       <c r="G103" s="20" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="H103" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="I103" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="E104" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="F104" s="47" t="s">
-        <v>64</v>
+        <v>118</v>
+      </c>
+      <c r="F104" s="46" t="s">
+        <v>63</v>
       </c>
       <c r="G104" s="20" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+      <c r="H104" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="I104" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="E105" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F105" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="G105" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="F105" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="G105" s="20" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="H105" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="I105" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="E106" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F106" s="36">
         <v>37897</v>
       </c>
       <c r="G106" s="20" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+      <c r="H106" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="I106" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
       <c r="E107" s="39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F107" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G107" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="H107" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="I107" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="E108" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F108" t="s">
+        <v>68</v>
+      </c>
+      <c r="G108" s="20" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="E108" s="20" t="s">
+      <c r="H108" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="I108" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="E109" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="F109" t="s">
         <v>72</v>
       </c>
-      <c r="F108" t="s">
-        <v>69</v>
-      </c>
-      <c r="G108" s="20" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="E109" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="F109" t="s">
-        <v>73</v>
-      </c>
       <c r="G109" s="20" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+      <c r="H109" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="I109" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E110" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="F110" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="F110" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="G110" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="G110" s="39" t="s">
+      <c r="H110" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="I110" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="E111" s="45" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="E111" s="46" t="s">
+      <c r="G111" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="G111" s="39" t="s">
+      <c r="H111" s="39" t="s">
+        <v>161</v>
+      </c>
+      <c r="I111" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="E112" s="20" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="E112" s="20" t="s">
+      <c r="G112" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="G112" s="20" t="s">
+      <c r="H112" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="I112" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E113" s="39" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="E113" s="39" t="s">
-        <v>165</v>
       </c>
       <c r="F113">
         <v>9876543210</v>
       </c>
       <c r="G113" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="H113" t="s">
+        <v>184</v>
+      </c>
+      <c r="I113" s="49" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="E114" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="F114" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G114" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="H114" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I114" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="E114" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="F114" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G114" s="20" t="s">
+      <c r="B115" s="13" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
-        <v>167</v>
-      </c>
-      <c r="B115" s="13" t="s">
-        <v>59</v>
       </c>
       <c r="C115" s="34">
         <v>12</v>
       </c>
       <c r="D115" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E115" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F115" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G115" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H115" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="I115" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="E116" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="E115" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="F115" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="G115" s="20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="E116" s="20" t="s">
+      <c r="F116" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="F116" s="35" t="s">
-        <v>62</v>
-      </c>
       <c r="G116" s="20" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="H116" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="I116" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="E117" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="F117" s="47" t="s">
-        <v>64</v>
+        <v>118</v>
+      </c>
+      <c r="F117" s="46" t="s">
+        <v>63</v>
       </c>
       <c r="G117" s="20" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+      <c r="H117" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="I117" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="E118" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F118" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="G118" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="F118" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="G118" s="20" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="H118" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="I118" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="E119" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F119" s="36">
         <v>37897</v>
       </c>
       <c r="G119" s="20" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+      <c r="H119" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="I119" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
       <c r="E120" s="39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F120" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G120" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="H120" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="I120" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="E121" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F121" t="s">
+        <v>68</v>
+      </c>
+      <c r="G121" s="20" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="E121" s="20" t="s">
+      <c r="H121" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="I121" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="E122" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="F122" t="s">
         <v>72</v>
       </c>
-      <c r="F121" t="s">
-        <v>69</v>
-      </c>
-      <c r="G121" s="20" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="E122" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="F122" t="s">
-        <v>73</v>
-      </c>
       <c r="G122" s="20" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+      <c r="H122" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="I122" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E123" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="F123" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="F123" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="G123" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="G123" s="39" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H123" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="I123" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E124" s="39" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F124">
         <v>9876543210</v>
       </c>
       <c r="G124" s="39" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+      <c r="H124" t="s">
+        <v>184</v>
+      </c>
+      <c r="I124" s="49" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E125" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="G125" s="39" t="s">
         <v>169</v>
       </c>
-      <c r="G125" s="39" t="s">
+      <c r="H125" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="I125" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E126" s="39" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="E126" s="39" t="s">
+      <c r="G126" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="G126" s="39" t="s">
+      <c r="H126" s="39" t="s">
+        <v>171</v>
+      </c>
+      <c r="I126" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E127" s="39" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E127" s="39" t="s">
+      <c r="G127" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="G127" s="39" t="s">
+      <c r="H127" s="39" t="s">
+        <v>173</v>
+      </c>
+      <c r="I127" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E128" s="39" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="E128" s="39" t="s">
+      <c r="G128" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="G128" s="39" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="H128" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="I128" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
       <c r="E129" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="F129" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G129" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="H129" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I129" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
         <v>179</v>
       </c>
-      <c r="F129" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G129" s="20" t="s">
+      <c r="B130" s="13" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
-        <v>180</v>
-      </c>
-      <c r="B130" s="13" t="s">
-        <v>59</v>
       </c>
       <c r="C130" s="34">
         <v>13</v>
       </c>
       <c r="D130" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E130" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F130" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G130" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H130" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="I130" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="E131" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="E130" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="F130" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="G130" s="20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="E131" s="20" t="s">
+      <c r="F131" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="F131" s="35" t="s">
-        <v>62</v>
-      </c>
       <c r="G131" s="20" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="H131" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="I131" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" ht="39.6" x14ac:dyDescent="0.3">
       <c r="E132" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="F132" s="47" t="s">
-        <v>64</v>
+        <v>118</v>
+      </c>
+      <c r="F132" s="46" t="s">
+        <v>63</v>
       </c>
       <c r="G132" s="20" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+      <c r="H132" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="I132" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" ht="39.6" x14ac:dyDescent="0.3">
       <c r="E133" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F133" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="G133" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="F133" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="G133" s="20" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="H133" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="I133" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" ht="39.6" x14ac:dyDescent="0.3">
       <c r="E134" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F134" s="36">
         <v>37897</v>
       </c>
       <c r="G134" s="20" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+      <c r="H134" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="I134" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
       <c r="E135" s="39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F135" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G135" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="H135" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="I135" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="E136" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F136" t="s">
+        <v>68</v>
+      </c>
+      <c r="G136" s="20" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="E136" s="20" t="s">
+      <c r="H136" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="I136" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="E137" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="F137" t="s">
         <v>72</v>
       </c>
-      <c r="F136" t="s">
-        <v>69</v>
-      </c>
-      <c r="G136" s="20" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="E137" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="F137" t="s">
-        <v>73</v>
-      </c>
       <c r="G137" s="20" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+      <c r="H137" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="I137" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E138" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="F138" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="F138" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="G138" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="G138" s="39" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H138" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="I138" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E139" s="39" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F139">
         <v>9876543210</v>
       </c>
       <c r="G139" s="39" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+      <c r="H139" t="s">
+        <v>184</v>
+      </c>
+      <c r="I139" s="49" t="s">
+        <v>182</v>
+      </c>
+      <c r="J139" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="E140" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="G140" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="G140" s="39" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="H140" s="39" t="s">
+        <v>181</v>
+      </c>
+      <c r="I140" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
       <c r="E141" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F141" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G141" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G141" s="20" t="s">
-        <v>58</v>
+      <c r="H141" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I141" s="48" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -4858,8 +5699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2C9D068-D540-454C-8DE6-9D8144402BBF}">
   <dimension ref="A1:L82"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView zoomScale="57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5827,44 +6668,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
     </row>
     <row r="3" spans="1:12" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="B3" s="55"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
     </row>
     <row r="4" spans="1:12" ht="25.8" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="58"/>
+      <c r="C4" s="58" t="s">
+        <v>210</v>
+      </c>
+      <c r="D4" s="59"/>
       <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2">
+        <v>45976</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="25.8" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="D5" s="3"/>
       <c r="E5" s="1"/>
       <c r="F5" s="2"/>
@@ -5873,8 +6720,10 @@
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="60"/>
-      <c r="D6" s="61"/>
+      <c r="C6" s="61" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="62"/>
       <c r="E6" s="1"/>
       <c r="F6" s="12"/>
     </row>
@@ -5923,13 +6772,23 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
+    <row r="10" spans="1:12" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="B10" t="s">
+        <v>184</v>
+      </c>
       <c r="C10" s="13"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="20"/>
+      <c r="D10" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>186</v>
+      </c>
       <c r="G10" s="29"/>
       <c r="H10" s="29"/>
       <c r="I10" s="29"/>
@@ -5941,8 +6800,12 @@
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="17"/>
+      <c r="D11" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>61</v>
+      </c>
       <c r="F11" s="20"/>
       <c r="G11" s="27"/>
       <c r="H11" s="27"/>
@@ -5955,8 +6818,12 @@
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="36"/>
+      <c r="D12" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="E12" s="40" t="s">
+        <v>63</v>
+      </c>
       <c r="F12" s="20"/>
       <c r="G12" s="27"/>
       <c r="H12" s="27"/>
@@ -5969,8 +6836,12 @@
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="17"/>
+      <c r="D13" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" s="40" t="s">
+        <v>63</v>
+      </c>
       <c r="F13" s="20"/>
       <c r="G13" s="28"/>
       <c r="H13" s="28"/>
@@ -5979,47 +6850,67 @@
       <c r="K13" s="28"/>
       <c r="L13" s="28"/>
     </row>
-    <row r="14" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="21"/>
+      <c r="D14" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="E14" s="36">
+        <v>37897</v>
+      </c>
       <c r="G14" s="21"/>
     </row>
     <row r="15" spans="1:12" s="9" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
+      <c r="D15" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>66</v>
+      </c>
       <c r="F15" s="17"/>
       <c r="G15" s="13"/>
     </row>
-    <row r="16" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A16" s="13"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
+      <c r="D16" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>68</v>
+      </c>
       <c r="F16" s="17"/>
       <c r="G16" s="13"/>
     </row>
-    <row r="17" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A17" s="13"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
+      <c r="D17" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>72</v>
+      </c>
       <c r="F17" s="18"/>
       <c r="G17" s="13"/>
     </row>
-    <row r="18" spans="1:7" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" s="9" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
+      <c r="D18" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>74</v>
+      </c>
       <c r="F18" s="22"/>
       <c r="G18" s="13"/>
     </row>
@@ -6027,8 +6918,12 @@
       <c r="A19" s="13"/>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
+      <c r="D19" t="s">
+        <v>184</v>
+      </c>
+      <c r="E19" s="13">
+        <v>9360416566</v>
+      </c>
       <c r="F19" s="22"/>
       <c r="G19" s="13"/>
     </row>
@@ -6483,8 +7378,13 @@
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C6:D6"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E14" r:id="rId1" display="bala123@gmail.com" xr:uid="{D93C151D-8055-4310-8B91-E9733604419D}"/>
+    <hyperlink ref="E11" r:id="rId2" xr:uid="{AD833405-84C7-43A3-A64B-146D34C14A27}"/>
+    <hyperlink ref="E18" r:id="rId3" xr:uid="{46EF147F-3296-42D8-B743-35F53BBB174F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -6492,8 +7392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:G32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6949,62 +7849,70 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
     </row>
     <row r="6" spans="2:7" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="55"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="62"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="63"/>
     </row>
     <row r="7" spans="2:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="57"/>
-      <c r="D7" s="58"/>
+      <c r="C7" s="58" t="s">
+        <v>210</v>
+      </c>
+      <c r="D7" s="59"/>
       <c r="E7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2">
+        <v>45976</v>
+      </c>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="2:7" ht="25.8" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="D8" s="3"/>
       <c r="E8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2">
+        <v>45698</v>
+      </c>
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="60"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="61"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="62"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
@@ -7027,99 +7935,197 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="10"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
+      <c r="B11" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>195</v>
+      </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="10"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
+      <c r="B12" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>195</v>
+      </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="10"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="9"/>
+      <c r="B13" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>195</v>
+      </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="10"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
+      <c r="B14" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>195</v>
+      </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="10"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
+      <c r="B15" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>195</v>
+      </c>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="10"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
+      <c r="B16" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>195</v>
+      </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="10"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
+      <c r="B17" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>195</v>
+      </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="10"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="9"/>
+      <c r="B18" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>195</v>
+      </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="10"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
+      <c r="B19" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>195</v>
+      </c>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
+      <c r="B20" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>195</v>
+      </c>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
+      <c r="B21" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>195</v>
+      </c>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
+      <c r="B22" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>185</v>
+      </c>
       <c r="G22" s="9"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">

</xml_diff>